<commit_message>
update medical speciality value set
</commit_message>
<xml_diff>
--- a/v0.7/ValueSet-medical-speciality-type-provider.xlsx
+++ b/v0.7/ValueSet-medical-speciality-type-provider.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="206">
   <si>
     <t>Property</t>
   </si>
@@ -114,268 +114,520 @@
     <t>http://hcp.org/codes/medical-specility-type-provider</t>
   </si>
   <si>
+    <t>general_medicine</t>
+  </si>
+  <si>
     <t>General Medicine</t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
+    <t>dental_surgery</t>
+  </si>
+  <si>
     <t>Dental surgery</t>
   </si>
   <si>
+    <t>nursing</t>
+  </si>
+  <si>
     <t>Nursing</t>
   </si>
   <si>
+    <t>pharmacy</t>
+  </si>
+  <si>
     <t>Pharmacy</t>
   </si>
   <si>
+    <t>nursing_midwifery</t>
+  </si>
+  <si>
     <t>Nursing Midwifery</t>
   </si>
   <si>
+    <t>military_surgeons</t>
+  </si>
+  <si>
     <t>Military surgeons</t>
   </si>
   <si>
+    <t>cardio_thoracic_and_vascular_surgery</t>
+  </si>
+  <si>
     <t>Cardio Thoracic and Vascular Surgery</t>
   </si>
   <si>
+    <t>cardiology</t>
+  </si>
+  <si>
     <t>Cardiology</t>
   </si>
   <si>
+    <t>allergy</t>
+  </si>
+  <si>
     <t>Allergy</t>
   </si>
   <si>
+    <t>chest_medicine</t>
+  </si>
+  <si>
     <t>Chest Medicine</t>
   </si>
   <si>
+    <t>clinical_psychology</t>
+  </si>
+  <si>
     <t>Clinical Psychology</t>
   </si>
   <si>
+    <t>cosmetic_dentistry</t>
+  </si>
+  <si>
     <t>Cosmetic Dentistry</t>
   </si>
   <si>
+    <t>cosmetic_surgery</t>
+  </si>
+  <si>
     <t>Cosmetic Surgery</t>
   </si>
   <si>
+    <t>endodontics</t>
+  </si>
+  <si>
     <t>Endodontics</t>
   </si>
   <si>
+    <t>ent</t>
+  </si>
+  <si>
     <t>ENT</t>
   </si>
   <si>
+    <t>critical_care</t>
+  </si>
+  <si>
     <t>Critical Care</t>
   </si>
   <si>
+    <t>dental_implants_and_cosmetic_dentistry</t>
+  </si>
+  <si>
     <t>Dental Implants &amp; Cosmetic Dentistry</t>
   </si>
   <si>
+    <t>dermatology_venereology_and_leprology</t>
+  </si>
+  <si>
     <t>Dermatology Venereology and Leprology</t>
   </si>
   <si>
+    <t>dermatology</t>
+  </si>
+  <si>
     <t>Dermatology</t>
   </si>
   <si>
+    <t>facial_plastic_surgery</t>
+  </si>
+  <si>
     <t>Facial Plastic Surgery</t>
   </si>
   <si>
+    <t>diabetology</t>
+  </si>
+  <si>
     <t>Diabetology</t>
   </si>
   <si>
+    <t>endocrinology</t>
+  </si>
+  <si>
     <t>Endocrinology</t>
   </si>
   <si>
+    <t>diet_and_nutrition</t>
+  </si>
+  <si>
     <t>Diet and Nutrition</t>
   </si>
   <si>
+    <t>diabetology_and_internal_medicine</t>
+  </si>
+  <si>
     <t>Diabetology &amp; Internal Medicine</t>
   </si>
   <si>
+    <t>gastrosurgery</t>
+  </si>
+  <si>
     <t>Gastrosurgery</t>
   </si>
   <si>
+    <t>gastroenterology</t>
+  </si>
+  <si>
     <t>Gastroenterology</t>
   </si>
   <si>
+    <t>general_surgery</t>
+  </si>
+  <si>
     <t>General Surgery</t>
   </si>
   <si>
+    <t>general_surgery_and_laparoscopic_surgery</t>
+  </si>
+  <si>
     <t>General Surgery &amp; Laparoscopic Surgery</t>
   </si>
   <si>
+    <t>gynecology_and_ultrasonology</t>
+  </si>
+  <si>
     <t>Gynecology &amp; Ultrasonology</t>
   </si>
   <si>
+    <t>head_and_neck_surgery</t>
+  </si>
+  <si>
     <t>Head &amp; Neck Surgery</t>
   </si>
   <si>
+    <t>head_and_neck_surgical_oncology</t>
+  </si>
+  <si>
     <t>Head &amp; Neck Surgical Oncology</t>
   </si>
   <si>
+    <t>hepato_pancreato_biliary_surgery</t>
+  </si>
+  <si>
     <t>Hepato Pancreato Biliary Surgery</t>
   </si>
   <si>
+    <t>infectious_disease_medicine</t>
+  </si>
+  <si>
     <t>Infectious Disease medicine</t>
   </si>
   <si>
+    <t>internal_medicine</t>
+  </si>
+  <si>
     <t>Internal Medicine</t>
   </si>
   <si>
-    <t>Internal Medicine &amp; Diabetics</t>
+    <t>neuro_surgery</t>
   </si>
   <si>
     <t>Neuro Surgery</t>
   </si>
   <si>
+    <t>resident_physicians</t>
+  </si>
+  <si>
     <t>Resident Physicians</t>
   </si>
   <si>
+    <t>respiratory_allergy_and_sleep_medicine</t>
+  </si>
+  <si>
     <t>Respiratory Allergy And Sleep Medicine</t>
   </si>
   <si>
+    <t>rheumatology</t>
+  </si>
+  <si>
     <t>Rheumatology</t>
   </si>
   <si>
+    <t>sexual_medicine</t>
+  </si>
+  <si>
     <t>Sexual Medicine</t>
   </si>
   <si>
+    <t>spine_surgery</t>
+  </si>
+  <si>
     <t>Spine Surgery</t>
   </si>
   <si>
+    <t>sports_medicine</t>
+  </si>
+  <si>
     <t>Sports Medicine</t>
   </si>
   <si>
+    <t>surgical_gastroenterology</t>
+  </si>
+  <si>
     <t>Surgical Gastroenterology</t>
   </si>
   <si>
+    <t>surgical_oncology</t>
+  </si>
+  <si>
     <t>Surgical Oncology</t>
   </si>
   <si>
+    <t>urology</t>
+  </si>
+  <si>
     <t>Urology</t>
   </si>
   <si>
+    <t>physiotherapy</t>
+  </si>
+  <si>
     <t>Physiotherapy</t>
   </si>
   <si>
+    <t>physiotherapy_and_rehabilitation</t>
+  </si>
+  <si>
     <t>Physiotherapy &amp; Rehabilitation</t>
   </si>
   <si>
+    <t>plastic_and_cosmetic_surgery</t>
+  </si>
+  <si>
     <t>Plastic and Cosmetic Surgery</t>
   </si>
   <si>
+    <t>plastic_surgery</t>
+  </si>
+  <si>
     <t>Plastic Surgery</t>
   </si>
   <si>
+    <t>podiatry</t>
+  </si>
+  <si>
     <t>Podiatry</t>
   </si>
   <si>
+    <t>prosthodontics_and_implants</t>
+  </si>
+  <si>
     <t>Prosthodontics &amp; Implants</t>
   </si>
   <si>
+    <t>psychiatry</t>
+  </si>
+  <si>
     <t>Psychiatry</t>
   </si>
   <si>
+    <t>pulmonology</t>
+  </si>
+  <si>
     <t>Pulmonology</t>
   </si>
   <si>
+    <t>radiation_oncology</t>
+  </si>
+  <si>
     <t>Radiation Oncology</t>
   </si>
   <si>
+    <t>radiology</t>
+  </si>
+  <si>
     <t>Radiology</t>
   </si>
   <si>
+    <t>laparoscopic_and_robotic_surgery</t>
+  </si>
+  <si>
     <t>Laparoscopic and Robotic Surgery</t>
   </si>
   <si>
+    <t>medical_gastroenterology</t>
+  </si>
+  <si>
     <t>Medical Gastroenterology</t>
   </si>
   <si>
+    <t>medical_oncology</t>
+  </si>
+  <si>
     <t>Medical Oncology</t>
   </si>
   <si>
+    <t>nephrology</t>
+  </si>
+  <si>
     <t>Nephrology</t>
   </si>
   <si>
+    <t>neurology</t>
+  </si>
+  <si>
     <t>Neurology</t>
   </si>
   <si>
+    <t>neurology_and_neuro_surgery</t>
+  </si>
+  <si>
     <t>Neurology &amp; Neuro Surgery</t>
   </si>
   <si>
+    <t>neuropsychiatry</t>
+  </si>
+  <si>
     <t>Neuropsychiatry</t>
   </si>
   <si>
-    <t>Neurosurgery</t>
+    <t>obstetrics_and_gynecology</t>
   </si>
   <si>
     <t>Obstetrics &amp; Gynecology</t>
   </si>
   <si>
+    <t>oncology</t>
+  </si>
+  <si>
     <t>Oncology</t>
   </si>
   <si>
+    <t>ophthalmology</t>
+  </si>
+  <si>
     <t>Ophthalmology</t>
   </si>
   <si>
+    <t>oral_and_maxillofacial_surgery</t>
+  </si>
+  <si>
     <t>Oral &amp; Maxillofacial Surgery</t>
   </si>
   <si>
+    <t>ortho_dontia</t>
+  </si>
+  <si>
     <t>Ortho Dontia</t>
   </si>
   <si>
+    <t>orthopedic_surgeon</t>
+  </si>
+  <si>
     <t>Orthopedic Surgeon</t>
   </si>
   <si>
+    <t>orthopedics</t>
+  </si>
+  <si>
     <t>Orthopedics</t>
   </si>
   <si>
+    <t>orthopedics_and_sports_medicine</t>
+  </si>
+  <si>
     <t>Orthopedics &amp; Sports Medicine</t>
   </si>
   <si>
+    <t>orthopedics_and_spine_surgery</t>
+  </si>
+  <si>
     <t>Orthopedics And Spine Surgery</t>
   </si>
   <si>
+    <t>orthopedics_and_upper_limb_surgery</t>
+  </si>
+  <si>
     <t>Orthopedics And Upper Limb Surgery</t>
   </si>
   <si>
+    <t>pediatric_endocrinology</t>
+  </si>
+  <si>
     <t>Pediatric Endocrinology</t>
   </si>
   <si>
+    <t>pediatric_ophthalmology_and_squint</t>
+  </si>
+  <si>
     <t>Pediatric Ophthalmology And Squint</t>
   </si>
   <si>
+    <t>paediatrics</t>
+  </si>
+  <si>
     <t>Paediatrics</t>
   </si>
   <si>
+    <t>paediatrics_and_neonatology</t>
+  </si>
+  <si>
     <t>Paediatrics &amp; Neonatology</t>
   </si>
   <si>
+    <t>paediatrics_nephrology</t>
+  </si>
+  <si>
     <t>Paediatrics - Nephrology</t>
   </si>
   <si>
+    <t>paediatrics_neurology</t>
+  </si>
+  <si>
     <t>Paediatrics - Neurology</t>
   </si>
   <si>
+    <t>paediatrics_surgery</t>
+  </si>
+  <si>
     <t>Paediatrics - Surgery</t>
   </si>
   <si>
+    <t>pathology</t>
+  </si>
+  <si>
     <t>Pathology</t>
   </si>
   <si>
+    <t>peadodontology_child_dentistry</t>
+  </si>
+  <si>
     <t>Peadodontology (Child Dentistry)</t>
   </si>
   <si>
+    <t>pediatric_pulmonology</t>
+  </si>
+  <si>
     <t>Pediatric Pulmonology</t>
   </si>
   <si>
+    <t>periodontia</t>
+  </si>
+  <si>
     <t>Periodontia</t>
   </si>
   <si>
+    <t>periodontology_and_implantology</t>
+  </si>
+  <si>
     <t>Periodontology and Implantology</t>
   </si>
   <si>
+    <t>peripheral_vascular_surgery</t>
+  </si>
+  <si>
     <t>Peripheral Vascular Surgery</t>
   </si>
   <si>
+    <t>physical_medicine_and_rehabilitation</t>
+  </si>
+  <si>
     <t>Physical Medicine &amp; Rehabilitation</t>
+  </si>
+  <si>
+    <t>physician_and_diabetology</t>
   </si>
   <si>
     <t>Physician &amp; Diabetology</t>
@@ -633,7 +885,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -670,15 +922,17 @@
         <v>32</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>33</v>
+      </c>
       <c r="E2" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -689,15 +943,17 @@
         <v>32</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" t="s" s="2">
+        <v>36</v>
+      </c>
       <c r="E3" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -708,15 +964,17 @@
         <v>32</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="E4" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -727,15 +985,17 @@
         <v>32</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="E5" t="s" s="2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -746,15 +1006,17 @@
         <v>32</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="E6" t="s" s="2">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -765,15 +1027,17 @@
         <v>32</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="E7" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -784,15 +1048,17 @@
         <v>32</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" t="s" s="2">
+        <v>46</v>
+      </c>
       <c r="E8" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -803,15 +1069,17 @@
         <v>32</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" t="s" s="2">
+        <v>48</v>
+      </c>
       <c r="E9" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -822,15 +1090,17 @@
         <v>32</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" t="s" s="2">
+        <v>50</v>
+      </c>
       <c r="E10" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -841,15 +1111,17 @@
         <v>32</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" t="s" s="2">
+        <v>52</v>
+      </c>
       <c r="E11" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
@@ -860,15 +1132,17 @@
         <v>32</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" t="s" s="2">
+        <v>54</v>
+      </c>
       <c r="E12" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -879,15 +1153,17 @@
         <v>32</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" t="s" s="2">
+        <v>56</v>
+      </c>
       <c r="E13" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -898,15 +1174,17 @@
         <v>32</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" t="s" s="2">
+        <v>58</v>
+      </c>
       <c r="E14" t="s" s="2">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -917,15 +1195,17 @@
         <v>32</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" t="s" s="2">
+        <v>60</v>
+      </c>
       <c r="E15" t="s" s="2">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -936,15 +1216,17 @@
         <v>32</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" t="s" s="2">
+        <v>62</v>
+      </c>
       <c r="E16" t="s" s="2">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -955,15 +1237,17 @@
         <v>32</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" t="s" s="2">
+        <v>64</v>
+      </c>
       <c r="E17" t="s" s="2">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -974,15 +1258,17 @@
         <v>32</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" t="s" s="2">
+        <v>66</v>
+      </c>
       <c r="E18" t="s" s="2">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -993,15 +1279,17 @@
         <v>32</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" t="s" s="2">
+        <v>68</v>
+      </c>
       <c r="E19" t="s" s="2">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
@@ -1012,15 +1300,17 @@
         <v>32</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="E20" t="s" s="2">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -1031,15 +1321,17 @@
         <v>32</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" t="s" s="2">
+        <v>72</v>
+      </c>
       <c r="E21" t="s" s="2">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
@@ -1050,15 +1342,17 @@
         <v>32</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="E22" t="s" s="2">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23">
@@ -1069,15 +1363,17 @@
         <v>32</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="E23" t="s" s="2">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24">
@@ -1088,15 +1384,17 @@
         <v>32</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="E24" t="s" s="2">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
@@ -1107,15 +1405,17 @@
         <v>32</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="E25" t="s" s="2">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
@@ -1126,15 +1426,17 @@
         <v>32</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" t="s" s="2">
+        <v>82</v>
+      </c>
       <c r="E26" t="s" s="2">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
@@ -1145,15 +1447,17 @@
         <v>32</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" t="s" s="2">
+        <v>84</v>
+      </c>
       <c r="E27" t="s" s="2">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
@@ -1164,15 +1468,17 @@
         <v>32</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" t="s" s="2">
+        <v>86</v>
+      </c>
       <c r="E28" t="s" s="2">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29">
@@ -1183,15 +1489,17 @@
         <v>32</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" t="s" s="2">
+        <v>88</v>
+      </c>
       <c r="E29" t="s" s="2">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30">
@@ -1202,15 +1510,17 @@
         <v>32</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" t="s" s="2">
+        <v>90</v>
+      </c>
       <c r="E30" t="s" s="2">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
@@ -1221,15 +1531,17 @@
         <v>32</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" t="s" s="2">
+        <v>92</v>
+      </c>
       <c r="E31" t="s" s="2">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32">
@@ -1240,15 +1552,17 @@
         <v>32</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" t="s" s="2">
+        <v>94</v>
+      </c>
       <c r="E32" t="s" s="2">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
@@ -1259,15 +1573,17 @@
         <v>32</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" t="s" s="2">
+        <v>96</v>
+      </c>
       <c r="E33" t="s" s="2">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -1278,15 +1594,17 @@
         <v>32</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="D34" t="s" s="2">
+        <v>98</v>
+      </c>
       <c r="E34" t="s" s="2">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35">
@@ -1297,15 +1615,17 @@
         <v>32</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" t="s" s="2">
+        <v>100</v>
+      </c>
       <c r="E35" t="s" s="2">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36">
@@ -1316,15 +1636,17 @@
         <v>32</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" t="s" s="2">
+        <v>102</v>
+      </c>
       <c r="E36" t="s" s="2">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37">
@@ -1335,15 +1657,17 @@
         <v>32</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="D37" t="s" s="2">
+        <v>104</v>
+      </c>
       <c r="E37" t="s" s="2">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38">
@@ -1354,15 +1678,17 @@
         <v>32</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="D38" t="s" s="2">
+        <v>106</v>
+      </c>
       <c r="E38" t="s" s="2">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39">
@@ -1373,15 +1699,17 @@
         <v>32</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="E39" t="s" s="2">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40">
@@ -1392,15 +1720,17 @@
         <v>32</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="D40" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="E40" t="s" s="2">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41">
@@ -1411,15 +1741,17 @@
         <v>32</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="D41" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="E41" t="s" s="2">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42">
@@ -1430,15 +1762,17 @@
         <v>32</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="E42" t="s" s="2">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43">
@@ -1449,15 +1783,17 @@
         <v>32</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="D43" t="s" s="2">
+        <v>116</v>
+      </c>
       <c r="E43" t="s" s="2">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44">
@@ -1468,15 +1804,17 @@
         <v>32</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="D44" t="s" s="2">
+        <v>118</v>
+      </c>
       <c r="E44" t="s" s="2">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45">
@@ -1487,15 +1825,17 @@
         <v>32</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="D45" t="s" s="2">
+        <v>120</v>
+      </c>
       <c r="E45" t="s" s="2">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46">
@@ -1506,15 +1846,17 @@
         <v>32</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="D46" t="s" s="2">
+        <v>122</v>
+      </c>
       <c r="E46" t="s" s="2">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47">
@@ -1525,15 +1867,17 @@
         <v>32</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="D47" t="s" s="2">
+        <v>124</v>
+      </c>
       <c r="E47" t="s" s="2">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48">
@@ -1544,15 +1888,17 @@
         <v>32</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="D48" t="s" s="2">
+        <v>126</v>
+      </c>
       <c r="E48" t="s" s="2">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49">
@@ -1563,15 +1909,17 @@
         <v>32</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="D49" t="s" s="2">
+        <v>128</v>
+      </c>
       <c r="E49" t="s" s="2">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50">
@@ -1582,15 +1930,17 @@
         <v>32</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="D50" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="E50" t="s" s="2">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
@@ -1601,15 +1951,17 @@
         <v>32</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="D51" t="s" s="2">
+        <v>132</v>
+      </c>
       <c r="E51" t="s" s="2">
-        <v>82</v>
+        <v>133</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52">
@@ -1620,15 +1972,17 @@
         <v>32</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="D52" t="s" s="2">
+        <v>134</v>
+      </c>
       <c r="E52" t="s" s="2">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53">
@@ -1639,15 +1993,17 @@
         <v>32</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="D53" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="E53" t="s" s="2">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54">
@@ -1658,15 +2014,17 @@
         <v>32</v>
       </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="D54" t="s" s="2">
+        <v>138</v>
+      </c>
       <c r="E54" t="s" s="2">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55">
@@ -1677,15 +2035,17 @@
         <v>32</v>
       </c>
       <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="D55" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="E55" t="s" s="2">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56">
@@ -1696,15 +2056,17 @@
         <v>32</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="D56" t="s" s="2">
+        <v>142</v>
+      </c>
       <c r="E56" t="s" s="2">
-        <v>87</v>
+        <v>143</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57">
@@ -1715,15 +2077,17 @@
         <v>32</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="D57" t="s" s="2">
+        <v>144</v>
+      </c>
       <c r="E57" t="s" s="2">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58">
@@ -1734,15 +2098,17 @@
         <v>32</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="D58" t="s" s="2">
+        <v>146</v>
+      </c>
       <c r="E58" t="s" s="2">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59">
@@ -1753,15 +2119,17 @@
         <v>32</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="D59" t="s" s="2">
+        <v>148</v>
+      </c>
       <c r="E59" t="s" s="2">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60">
@@ -1772,15 +2140,17 @@
         <v>32</v>
       </c>
       <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="D60" t="s" s="2">
+        <v>150</v>
+      </c>
       <c r="E60" t="s" s="2">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61">
@@ -1791,15 +2161,17 @@
         <v>32</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="D61" t="s" s="2">
+        <v>152</v>
+      </c>
       <c r="E61" t="s" s="2">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62">
@@ -1810,15 +2182,17 @@
         <v>32</v>
       </c>
       <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="D62" t="s" s="2">
+        <v>154</v>
+      </c>
       <c r="E62" t="s" s="2">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63">
@@ -1829,15 +2203,17 @@
         <v>32</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="D63" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="E63" t="s" s="2">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G63" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64">
@@ -1848,15 +2224,17 @@
         <v>32</v>
       </c>
       <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="D64" t="s" s="2">
+        <v>158</v>
+      </c>
       <c r="E64" t="s" s="2">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65">
@@ -1867,15 +2245,17 @@
         <v>32</v>
       </c>
       <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="D65" t="s" s="2">
+        <v>160</v>
+      </c>
       <c r="E65" t="s" s="2">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G65" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66">
@@ -1886,15 +2266,17 @@
         <v>32</v>
       </c>
       <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="D66" t="s" s="2">
+        <v>162</v>
+      </c>
       <c r="E66" t="s" s="2">
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67">
@@ -1905,15 +2287,17 @@
         <v>32</v>
       </c>
       <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="D67" t="s" s="2">
+        <v>164</v>
+      </c>
       <c r="E67" t="s" s="2">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68">
@@ -1924,15 +2308,17 @@
         <v>32</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="D68" t="s" s="2">
+        <v>166</v>
+      </c>
       <c r="E68" t="s" s="2">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69">
@@ -1943,15 +2329,17 @@
         <v>32</v>
       </c>
       <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="D69" t="s" s="2">
+        <v>168</v>
+      </c>
       <c r="E69" t="s" s="2">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70">
@@ -1962,15 +2350,17 @@
         <v>32</v>
       </c>
       <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="D70" t="s" s="2">
+        <v>170</v>
+      </c>
       <c r="E70" t="s" s="2">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71">
@@ -1981,15 +2371,17 @@
         <v>32</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="D71" t="s" s="2">
+        <v>172</v>
+      </c>
       <c r="E71" t="s" s="2">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G71" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72">
@@ -2000,15 +2392,17 @@
         <v>32</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="D72" t="s" s="2">
+        <v>174</v>
+      </c>
       <c r="E72" t="s" s="2">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73">
@@ -2019,15 +2413,17 @@
         <v>32</v>
       </c>
       <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="D73" t="s" s="2">
+        <v>176</v>
+      </c>
       <c r="E73" t="s" s="2">
-        <v>104</v>
+        <v>177</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74">
@@ -2038,15 +2434,17 @@
         <v>32</v>
       </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="D74" t="s" s="2">
+        <v>178</v>
+      </c>
       <c r="E74" t="s" s="2">
-        <v>105</v>
+        <v>179</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75">
@@ -2057,15 +2455,17 @@
         <v>32</v>
       </c>
       <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="D75" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="E75" t="s" s="2">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76">
@@ -2076,15 +2476,17 @@
         <v>32</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="D76" t="s" s="2">
+        <v>182</v>
+      </c>
       <c r="E76" t="s" s="2">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77">
@@ -2095,15 +2497,17 @@
         <v>32</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="D77" t="s" s="2">
+        <v>184</v>
+      </c>
       <c r="E77" t="s" s="2">
-        <v>108</v>
+        <v>185</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78">
@@ -2114,15 +2518,17 @@
         <v>32</v>
       </c>
       <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="D78" t="s" s="2">
+        <v>186</v>
+      </c>
       <c r="E78" t="s" s="2">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="79">
@@ -2133,15 +2539,17 @@
         <v>32</v>
       </c>
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="D79" t="s" s="2">
+        <v>188</v>
+      </c>
       <c r="E79" t="s" s="2">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G79" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80">
@@ -2152,15 +2560,17 @@
         <v>32</v>
       </c>
       <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="D80" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="E80" t="s" s="2">
-        <v>111</v>
+        <v>191</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81">
@@ -2171,15 +2581,17 @@
         <v>32</v>
       </c>
       <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="D81" t="s" s="2">
+        <v>192</v>
+      </c>
       <c r="E81" t="s" s="2">
-        <v>112</v>
+        <v>193</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82">
@@ -2190,15 +2602,17 @@
         <v>32</v>
       </c>
       <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="D82" t="s" s="2">
+        <v>194</v>
+      </c>
       <c r="E82" t="s" s="2">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83">
@@ -2209,15 +2623,17 @@
         <v>32</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="D83" t="s" s="2">
+        <v>196</v>
+      </c>
       <c r="E83" t="s" s="2">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84">
@@ -2228,15 +2644,17 @@
         <v>32</v>
       </c>
       <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="D84" t="s" s="2">
+        <v>198</v>
+      </c>
       <c r="E84" t="s" s="2">
-        <v>115</v>
+        <v>199</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="85">
@@ -2247,15 +2665,17 @@
         <v>32</v>
       </c>
       <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="D85" t="s" s="2">
+        <v>200</v>
+      </c>
       <c r="E85" t="s" s="2">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86">
@@ -2266,15 +2686,17 @@
         <v>32</v>
       </c>
       <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="D86" t="s" s="2">
+        <v>202</v>
+      </c>
       <c r="E86" t="s" s="2">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="F86" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G86" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87">
@@ -2285,72 +2707,17 @@
         <v>32</v>
       </c>
       <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="D87" t="s" s="2">
+        <v>204</v>
+      </c>
       <c r="E87" t="s" s="2">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="F87" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B88" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="F88" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="G88" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B89" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="F89" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="G89" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B90" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="F90" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="G90" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>